<commit_message>
Added the velocity merger
</commit_message>
<xml_diff>
--- a/SpringMVC/doc/User Stories.xlsx
+++ b/SpringMVC/doc/User Stories.xlsx
@@ -4,19 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="21030" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$B$3:$E$7</definedName>
+  </definedNames>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Epic</t>
   </si>
@@ -43,6 +47,15 @@
   </si>
   <si>
     <t>SP</t>
+  </si>
+  <si>
+    <t>Als Administrator benötige ich die Möglichkeit Templates zu benutzen und Templates mit Daten zu mergen.</t>
+  </si>
+  <si>
+    <t>Als Technik möchte ich auf einfache Art und Weise Templates, die im Class-Path liegen mit Property Dateien mergen, damit ich verschiedene die Templates verschieden nutzen kann.</t>
+  </si>
+  <si>
+    <t>Open</t>
   </si>
 </sst>
 </file>
@@ -429,17 +442,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E5"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="B3:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="140" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="4" max="4" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -456,7 +470,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
@@ -467,7 +481,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
@@ -481,7 +495,37 @@
         <v>2</v>
       </c>
     </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <autoFilter ref="B3:E7">
+    <filterColumn colId="2">
+      <filters blank="1">
+        <filter val="Open"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>